<commit_message>
added a vi to manage the shooting, and to adjust the cannon's motors and angle. added a function that prevents a frisbee to enter the cannon (from the flipper) while shooting. added Freeze Value.vi to the VI Toolkit (this vi freezes a value on command). modified the Exit info list.xlsx to include all of the used refnum names.
Some of these codes haven't been tested yet...
</commit_message>
<xml_diff>
--- a/ king-kong-2230-2013/Documents/Exit info list.xlsx
+++ b/ king-kong-2230-2013/Documents/Exit info list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
   <si>
     <t>Begin</t>
   </si>
@@ -232,6 +232,39 @@
   </si>
   <si>
     <t>bool</t>
+  </si>
+  <si>
+    <t>refnum name</t>
+  </si>
+  <si>
+    <t>Disc Out</t>
+  </si>
+  <si>
+    <t>CannonAI</t>
+  </si>
+  <si>
+    <t>Cannon</t>
+  </si>
+  <si>
+    <t>InFlipper</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>FlipperAtPlace</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>FrisbeeDirection</t>
+  </si>
+  <si>
+    <t>driver's joystick</t>
+  </si>
+  <si>
+    <t>operator's joystick</t>
   </si>
 </sst>
 </file>
@@ -580,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -934,12 +967,146 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:D24"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.375" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added a vi that receives data from the dashboard to the robot, and updates it in the Get Dashboard Data.vi. modified the Exit info list.xlsx, and the Begin.vi
</commit_message>
<xml_diff>
--- a/ king-kong-2230-2013/Documents/Exit info list.xlsx
+++ b/ king-kong-2230-2013/Documents/Exit info list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="94">
   <si>
     <t>Begin</t>
   </si>
@@ -237,9 +237,6 @@
     <t>refnum name</t>
   </si>
   <si>
-    <t>Disc Out</t>
-  </si>
-  <si>
     <t>CannonAI</t>
   </si>
   <si>
@@ -265,6 +262,42 @@
   </si>
   <si>
     <t>operator's joystick</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t>PWM 10</t>
+  </si>
+  <si>
+    <t>DIO 6</t>
+  </si>
+  <si>
+    <t>DIO 7-8</t>
+  </si>
+  <si>
+    <t>zAvit</t>
+  </si>
+  <si>
+    <t>Jaguar Motor</t>
+  </si>
+  <si>
+    <t>measures shooting motor's RPM</t>
+  </si>
+  <si>
+    <t>measures angle of cannon</t>
+  </si>
+  <si>
+    <t>cannon angle</t>
+  </si>
+  <si>
+    <t>outer shooting cannon</t>
+  </si>
+  <si>
+    <t>inner shooting cannon</t>
+  </si>
+  <si>
+    <t>flipper's motor</t>
   </si>
 </sst>
 </file>
@@ -967,17 +1000,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D24"/>
+  <dimension ref="A2:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.375" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1016,7 +1049,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1030,7 +1063,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1040,70 +1073,183 @@
       <c r="A8" t="s">
         <v>24</v>
       </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>86</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>48</v>
       </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>80</v>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>